<commit_message>
Modified outputTest so that we no longer use a copy of output.m. Also modified variable names in the medium-scale networks
</commit_message>
<xml_diff>
--- a/test_files/data_samples/22-genes_47-edges_Dahlquist-data_Sigmoidal_forward_graph.xlsx
+++ b/test_files/data_samples/22-genes_47-edges_Dahlquist-data_Sigmoidal_forward_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="0" windowWidth="25095" windowHeight="13365" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="1635" yWindow="0" windowWidth="25095" windowHeight="13365"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" r:id="rId1"/>
@@ -16,23 +16,12 @@
     <sheet name="optimization_parameters" sheetId="9" r:id="rId7"/>
     <sheet name="threshold_b" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="47">
-  <si>
-    <t>StandardName</t>
-  </si>
-  <si>
-    <t>production_rates</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="47">
   <si>
     <t>ACE2</t>
   </si>
@@ -100,12 +89,6 @@
     <t>ZAP1</t>
   </si>
   <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
-    <t>DegradationRate</t>
-  </si>
-  <si>
     <t>optimization_parameter</t>
   </si>
   <si>
@@ -168,12 +151,24 @@
   <si>
     <t>id</t>
   </si>
+  <si>
+    <t>regulators/controllers</t>
+  </si>
+  <si>
+    <t>threshold_b</t>
+  </si>
+  <si>
+    <t>degradation_rate</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +180,10 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,21 +203,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -519,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -527,15 +533,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0.46209812037329684</v>
@@ -543,7 +549,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>5.436448474979963E-2</v>
@@ -551,7 +557,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>5.436448474979963E-2</v>
@@ -559,7 +565,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>5.3319013889226559E-2</v>
@@ -567,7 +573,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5.436448474979963E-2</v>
@@ -575,7 +581,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0.46209812037329684</v>
@@ -583,7 +589,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>5.436448474979963E-2</v>
@@ -591,7 +597,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>5.4364483999999998E-2</v>
@@ -599,7 +605,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>9.2419624074659368E-2</v>
@@ -607,7 +613,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0.69314718055994529</v>
@@ -615,7 +621,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>5.436448474979963E-2</v>
@@ -623,7 +629,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>5.4364483999999998E-2</v>
@@ -631,7 +637,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>5.4364483999999998E-2</v>
@@ -639,7 +645,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>9.2419624074659368E-2</v>
@@ -647,7 +653,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>5.4364483999999998E-2</v>
@@ -655,7 +661,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>3.7467415165402446E-2</v>
@@ -663,7 +669,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>9.8318749015595085E-3</v>
@@ -671,7 +677,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>5.436448474979963E-2</v>
@@ -679,7 +685,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0.46209812037329684</v>
@@ -687,7 +693,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>5.5451774444795626E-2</v>
@@ -695,7 +701,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0.46209812037329684</v>
@@ -703,7 +709,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>8.504873381103624E-3</v>
@@ -724,22 +730,22 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0.23104906018664842</v>
@@ -747,7 +753,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2.7182242374899815E-2</v>
@@ -755,7 +761,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2.7182242374899815E-2</v>
@@ -763,7 +769,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2.6659506944613279E-2</v>
@@ -771,7 +777,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2.7182242374899815E-2</v>
@@ -779,7 +785,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0.23104906018664842</v>
@@ -787,7 +793,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2.7182242374899815E-2</v>
@@ -795,7 +801,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2.7182241999999999E-2</v>
@@ -803,7 +809,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>4.6209812037329684E-2</v>
@@ -811,7 +817,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0.34657359027997264</v>
@@ -819,7 +825,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2.7182242374899815E-2</v>
@@ -827,7 +833,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>2.7182241999999999E-2</v>
@@ -835,7 +841,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2.7182241999999999E-2</v>
@@ -843,7 +849,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>4.6209812037329684E-2</v>
@@ -851,7 +857,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>2.7182241999999999E-2</v>
@@ -859,7 +865,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1.8733707582701223E-2</v>
@@ -867,7 +873,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>4.9159374507797542E-3</v>
@@ -875,7 +881,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>2.7182242374899815E-2</v>
@@ -883,7 +889,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0.23104906018664842</v>
@@ -891,7 +897,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>2.7725887222397813E-2</v>
@@ -899,7 +905,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0.23104906018664842</v>
@@ -907,7 +913,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>4.252436690551812E-3</v>
@@ -927,15 +933,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3">
         <v>15</v>
@@ -979,7 +983,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0.61260000000000003</v>
@@ -1023,7 +1027,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>-2.3784999999999998</v>
@@ -1067,7 +1071,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-0.1336</v>
@@ -1111,7 +1115,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>-0.4622</v>
@@ -1155,7 +1159,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.52449999999999997</v>
@@ -1199,7 +1203,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>-1.2922</v>
@@ -1243,7 +1247,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0.54659999999999997</v>
@@ -1287,7 +1291,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0.30499999999999999</v>
@@ -1331,7 +1335,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3.2513999999999998</v>
@@ -1375,7 +1379,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>-1.0669</v>
@@ -1419,7 +1423,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>-2.5242</v>
@@ -1463,7 +1467,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>-0.51770000000000005</v>
@@ -1507,7 +1511,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>-0.77139999999999997</v>
@@ -1551,7 +1555,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3.5400000000000001E-2</v>
@@ -1595,7 +1599,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>-0.1419</v>
@@ -1639,7 +1643,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>-1.7149000000000001</v>
@@ -1683,7 +1687,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>-0.98409999999999997</v>
@@ -1727,7 +1731,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>-0.76890000000000003</v>
@@ -1771,7 +1775,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>-1.1019000000000001</v>
@@ -1815,7 +1819,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>-1.1738999999999999</v>
@@ -1859,7 +1863,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>-0.20730000000000001</v>
@@ -1903,7 +1907,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0.68720000000000003</v>
@@ -1959,15 +1963,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1">
         <v>15</v>
@@ -2008,7 +2010,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>-0.17730000000000001</v>
@@ -2049,7 +2051,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0.66379999999999995</v>
@@ -2090,7 +2092,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-0.68189999999999995</v>
@@ -2131,7 +2133,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2.52E-2</v>
@@ -2172,7 +2174,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>-0.31540000000000001</v>
@@ -2213,7 +2215,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0.93259999999999998</v>
@@ -2254,7 +2256,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>6.4299999999999996E-2</v>
@@ -2295,7 +2297,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>-0.879</v>
@@ -2336,7 +2338,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>4.8802000000000003</v>
@@ -2377,7 +2379,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0.85880000000000001</v>
@@ -2418,7 +2420,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>-0.62</v>
@@ -2459,7 +2461,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>-0.87529999999999997</v>
@@ -2500,7 +2502,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0.68100000000000005</v>
@@ -2541,7 +2543,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1.0706</v>
@@ -2582,7 +2584,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>-0.1585</v>
@@ -2623,7 +2625,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1.1978</v>
@@ -2664,7 +2666,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>-0.4597</v>
@@ -2705,7 +2707,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>-0.1303</v>
@@ -2746,7 +2748,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>-1.1979</v>
@@ -2787,7 +2789,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>-0.85289999999999999</v>
@@ -2828,7 +2830,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>-1.3436999999999999</v>
@@ -2869,7 +2871,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0.80800000000000005</v>
@@ -2922,86 +2924,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
+      <c r="A1" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3427,7 +3427,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3782,7 +3782,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3924,7 +3924,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3995,7 +3995,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4421,7 +4421,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4563,11 +4563,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4575,148 +4570,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
+      <c r="A1" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0</v>
-      </c>
-      <c r="V2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4">
         <v>0</v>
       </c>
       <c r="W2">
@@ -4725,69 +4718,69 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <v>0</v>
+      </c>
+      <c r="V3" s="4">
         <v>0</v>
       </c>
       <c r="W3">
@@ -4796,69 +4789,69 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4">
         <v>0</v>
       </c>
       <c r="W4">
@@ -4867,69 +4860,69 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="5">
-        <v>0</v>
-      </c>
-      <c r="T5" s="5">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5">
-        <v>0</v>
-      </c>
-      <c r="V5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <v>0</v>
+      </c>
+      <c r="V5" s="4">
         <v>0</v>
       </c>
       <c r="W5">
@@ -4938,69 +4931,69 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>0</v>
-      </c>
-      <c r="R6" s="5">
-        <v>0</v>
-      </c>
-      <c r="S6" s="5">
-        <v>0</v>
-      </c>
-      <c r="T6" s="5">
-        <v>0</v>
-      </c>
-      <c r="U6" s="5">
-        <v>0</v>
-      </c>
-      <c r="V6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4">
+        <v>0</v>
+      </c>
+      <c r="V6" s="4">
         <v>0</v>
       </c>
       <c r="W6">
@@ -5009,69 +5002,69 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
-        <v>0</v>
-      </c>
-      <c r="T7" s="5">
-        <v>1</v>
-      </c>
-      <c r="U7" s="5">
-        <v>0</v>
-      </c>
-      <c r="V7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0</v>
+      </c>
+      <c r="V7" s="4">
         <v>0</v>
       </c>
       <c r="W7">
@@ -5080,69 +5073,69 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>1</v>
-      </c>
-      <c r="R8" s="5">
-        <v>1</v>
-      </c>
-      <c r="S8" s="5">
-        <v>0</v>
-      </c>
-      <c r="T8" s="5">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5">
-        <v>0</v>
-      </c>
-      <c r="V8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+      <c r="V8" s="4">
         <v>0</v>
       </c>
       <c r="W8">
@@ -5151,69 +5144,69 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>0</v>
-      </c>
-      <c r="R9" s="5">
-        <v>0</v>
-      </c>
-      <c r="S9" s="5">
-        <v>0</v>
-      </c>
-      <c r="T9" s="5">
-        <v>0</v>
-      </c>
-      <c r="U9" s="5">
-        <v>0</v>
-      </c>
-      <c r="V9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0</v>
+      </c>
+      <c r="V9" s="4">
         <v>0</v>
       </c>
       <c r="W9">
@@ -5222,69 +5215,69 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5">
-        <v>0</v>
-      </c>
-      <c r="V10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0</v>
+      </c>
+      <c r="V10" s="4">
         <v>0</v>
       </c>
       <c r="W10">
@@ -5293,69 +5286,69 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
-      <c r="S11" s="5">
-        <v>0</v>
-      </c>
-      <c r="T11" s="5">
-        <v>0</v>
-      </c>
-      <c r="U11" s="5">
-        <v>0</v>
-      </c>
-      <c r="V11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0</v>
+      </c>
+      <c r="V11" s="4">
         <v>0</v>
       </c>
       <c r="W11">
@@ -5364,69 +5357,69 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <v>0</v>
-      </c>
-      <c r="N12" s="5">
-        <v>0</v>
-      </c>
-      <c r="O12" s="5">
-        <v>0</v>
-      </c>
-      <c r="P12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>0</v>
-      </c>
-      <c r="R12" s="5">
-        <v>1</v>
-      </c>
-      <c r="S12" s="5">
-        <v>0</v>
-      </c>
-      <c r="T12" s="5">
-        <v>0</v>
-      </c>
-      <c r="U12" s="5">
-        <v>0</v>
-      </c>
-      <c r="V12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <v>0</v>
+      </c>
+      <c r="V12" s="4">
         <v>0</v>
       </c>
       <c r="W12">
@@ -5435,69 +5428,69 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0</v>
-      </c>
-      <c r="L13" s="5">
-        <v>0</v>
-      </c>
-      <c r="M13" s="5">
-        <v>0</v>
-      </c>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
-      <c r="O13" s="5">
-        <v>0</v>
-      </c>
-      <c r="P13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>0</v>
-      </c>
-      <c r="R13" s="5">
-        <v>0</v>
-      </c>
-      <c r="S13" s="5">
-        <v>0</v>
-      </c>
-      <c r="T13" s="5">
-        <v>0</v>
-      </c>
-      <c r="U13" s="5">
-        <v>0</v>
-      </c>
-      <c r="V13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4">
+        <v>0</v>
+      </c>
+      <c r="V13" s="4">
         <v>0</v>
       </c>
       <c r="W13">
@@ -5506,69 +5499,69 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1</v>
-      </c>
-      <c r="K14" s="5">
-        <v>0</v>
-      </c>
-      <c r="L14" s="5">
-        <v>0</v>
-      </c>
-      <c r="M14" s="5">
-        <v>0</v>
-      </c>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-      <c r="O14" s="5">
-        <v>0</v>
-      </c>
-      <c r="P14" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>0</v>
-      </c>
-      <c r="R14" s="5">
-        <v>0</v>
-      </c>
-      <c r="S14" s="5">
-        <v>0</v>
-      </c>
-      <c r="T14" s="5">
-        <v>0</v>
-      </c>
-      <c r="U14" s="5">
-        <v>0</v>
-      </c>
-      <c r="V14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0</v>
+      </c>
+      <c r="T14" s="4">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0</v>
+      </c>
+      <c r="V14" s="4">
         <v>0</v>
       </c>
       <c r="W14">
@@ -5577,69 +5570,69 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>1</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>0</v>
-      </c>
-      <c r="P15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>1</v>
-      </c>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
-      <c r="S15" s="5">
-        <v>0</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0</v>
-      </c>
-      <c r="U15" s="5">
-        <v>0</v>
-      </c>
-      <c r="V15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0</v>
+      </c>
+      <c r="V15" s="4">
         <v>0</v>
       </c>
       <c r="W15">
@@ -5648,69 +5641,69 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <v>1</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5">
-        <v>0</v>
-      </c>
-      <c r="M16" s="5">
-        <v>0</v>
-      </c>
-      <c r="N16" s="5">
-        <v>0</v>
-      </c>
-      <c r="O16" s="5">
-        <v>0</v>
-      </c>
-      <c r="P16" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>0</v>
-      </c>
-      <c r="R16" s="5">
-        <v>0</v>
-      </c>
-      <c r="S16" s="5">
-        <v>0</v>
-      </c>
-      <c r="T16" s="5">
-        <v>0</v>
-      </c>
-      <c r="U16" s="5">
-        <v>0</v>
-      </c>
-      <c r="V16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+      <c r="V16" s="4">
         <v>0</v>
       </c>
       <c r="W16">
@@ -5719,69 +5712,69 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>0</v>
-      </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5">
-        <v>0</v>
-      </c>
-      <c r="S17" s="5">
-        <v>0</v>
-      </c>
-      <c r="T17" s="5">
-        <v>0</v>
-      </c>
-      <c r="U17" s="5">
-        <v>0</v>
-      </c>
-      <c r="V17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>0</v>
+      </c>
+      <c r="V17" s="4">
         <v>0</v>
       </c>
       <c r="W17">
@@ -5790,69 +5783,69 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5">
-        <v>0</v>
-      </c>
-      <c r="O18" s="5">
-        <v>0</v>
-      </c>
-      <c r="P18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="5">
-        <v>0</v>
-      </c>
-      <c r="R18" s="5">
-        <v>0</v>
-      </c>
-      <c r="S18" s="5">
-        <v>0</v>
-      </c>
-      <c r="T18" s="5">
-        <v>0</v>
-      </c>
-      <c r="U18" s="5">
-        <v>0</v>
-      </c>
-      <c r="V18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+      <c r="V18" s="4">
         <v>0</v>
       </c>
       <c r="W18">
@@ -5861,69 +5854,69 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
-        <v>0</v>
-      </c>
-      <c r="M19" s="5">
-        <v>0</v>
-      </c>
-      <c r="N19" s="5">
-        <v>0</v>
-      </c>
-      <c r="O19" s="5">
-        <v>1</v>
-      </c>
-      <c r="P19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>0</v>
-      </c>
-      <c r="R19" s="5">
-        <v>0</v>
-      </c>
-      <c r="S19" s="5">
-        <v>0</v>
-      </c>
-      <c r="T19" s="5">
-        <v>0</v>
-      </c>
-      <c r="U19" s="5">
-        <v>0</v>
-      </c>
-      <c r="V19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <v>0</v>
+      </c>
+      <c r="V19" s="4">
         <v>0</v>
       </c>
       <c r="W19">
@@ -5932,69 +5925,69 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>1</v>
-      </c>
-      <c r="L20" s="5">
-        <v>0</v>
-      </c>
-      <c r="M20" s="5">
-        <v>0</v>
-      </c>
-      <c r="N20" s="5">
-        <v>0</v>
-      </c>
-      <c r="O20" s="5">
-        <v>0</v>
-      </c>
-      <c r="P20" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>0</v>
-      </c>
-      <c r="R20" s="5">
-        <v>1</v>
-      </c>
-      <c r="S20" s="5">
-        <v>0</v>
-      </c>
-      <c r="T20" s="5">
-        <v>0</v>
-      </c>
-      <c r="U20" s="5">
-        <v>0</v>
-      </c>
-      <c r="V20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
+        <v>1</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+      <c r="V20" s="4">
         <v>0</v>
       </c>
       <c r="W20">
@@ -6003,69 +5996,69 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="5">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
-        <v>1</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
-        <v>1</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0</v>
-      </c>
-      <c r="M21" s="5">
-        <v>0</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0</v>
-      </c>
-      <c r="P21" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>0</v>
-      </c>
-      <c r="R21" s="5">
-        <v>0</v>
-      </c>
-      <c r="S21" s="5">
-        <v>0</v>
-      </c>
-      <c r="T21" s="5">
-        <v>0</v>
-      </c>
-      <c r="U21" s="5">
-        <v>0</v>
-      </c>
-      <c r="V21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0</v>
+      </c>
+      <c r="S21" s="4">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4">
+        <v>0</v>
+      </c>
+      <c r="V21" s="4">
         <v>0</v>
       </c>
       <c r="W21">
@@ -6074,69 +6067,69 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
-        <v>1</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>1</v>
-      </c>
-      <c r="L22" s="5">
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <v>0</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>0</v>
-      </c>
-      <c r="R22" s="5">
-        <v>1</v>
-      </c>
-      <c r="S22" s="5">
-        <v>0</v>
-      </c>
-      <c r="T22" s="5">
-        <v>0</v>
-      </c>
-      <c r="U22" s="5">
-        <v>0</v>
-      </c>
-      <c r="V22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4">
+        <v>1</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0</v>
+      </c>
+      <c r="T22" s="4">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
+        <v>0</v>
+      </c>
+      <c r="V22" s="4">
         <v>0</v>
       </c>
       <c r="W22">
@@ -6145,69 +6138,69 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
-        <v>0</v>
-      </c>
-      <c r="L23" s="5">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0</v>
-      </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-      <c r="O23" s="5">
-        <v>0</v>
-      </c>
-      <c r="P23" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>0</v>
-      </c>
-      <c r="R23" s="5">
-        <v>0</v>
-      </c>
-      <c r="S23" s="5">
-        <v>0</v>
-      </c>
-      <c r="T23" s="5">
-        <v>0</v>
-      </c>
-      <c r="U23" s="5">
-        <v>0</v>
-      </c>
-      <c r="V23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4">
+        <v>0</v>
+      </c>
+      <c r="S23" s="4">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4">
+        <v>0</v>
+      </c>
+      <c r="U23" s="4">
+        <v>0</v>
+      </c>
+      <c r="V23" s="4">
         <v>0</v>
       </c>
       <c r="W23">
@@ -6216,11 +6209,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6229,7 +6217,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6238,118 +6226,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
+      <c r="A1" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
+      <c r="A2" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
+      <c r="A3" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
+      <c r="A4" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
+      <c r="A5" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
+      <c r="A6" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
+      <c r="A7" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="6">
+      <c r="A10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="6">
+      <c r="A11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="A13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5">
         <v>15</v>
       </c>
       <c r="C13">
@@ -6360,21 +6348,21 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
+      <c r="A14" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="7">
+      <c r="A15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="6">
         <v>3</v>
       </c>
       <c r="C15">
@@ -6382,10 +6370,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7">
+      <c r="A16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="6">
         <v>0</v>
       </c>
       <c r="C16">
@@ -6393,8 +6381,8 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
+      <c r="A17" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -6438,11 +6426,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6450,20 +6433,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
+      <c r="A1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6471,7 +6460,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6479,7 +6468,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6487,7 +6476,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6495,7 +6484,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6503,7 +6492,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6511,7 +6500,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6519,7 +6508,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6527,7 +6516,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6535,7 +6524,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6543,7 +6532,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6551,7 +6540,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6559,7 +6548,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6567,7 +6556,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -6575,7 +6564,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -6583,7 +6572,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -6591,7 +6580,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -6599,7 +6588,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -6607,7 +6596,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -6615,7 +6604,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -6623,7 +6612,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -6631,7 +6620,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -6639,10 +6628,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed input sheet and removed .mat file that was hanging around matlab_codes folder
</commit_message>
<xml_diff>
--- a/test_files/data_samples/22-genes_47-edges_Dahlquist-data_Sigmoidal_forward_graph.xlsx
+++ b/test_files/data_samples/22-genes_47-edges_Dahlquist-data_Sigmoidal_forward_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="0" windowWidth="25095" windowHeight="13365" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="1635" yWindow="0" windowWidth="25095" windowHeight="13365"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="48">
   <si>
     <t>ACE2</t>
   </si>
@@ -158,20 +158,20 @@
     <t>production_rate</t>
   </si>
   <si>
-    <t>targets/regulators</t>
-  </si>
-  <si>
     <t>production_function</t>
   </si>
   <si>
     <t>L_curve</t>
+  </si>
+  <si>
+    <t>cols regulators/rows targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +187,12 @@
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,11 +225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2927,13 +2932,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>45</v>
+    <row r="1" spans="1:23" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4577,9 +4584,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>45</v>
+    <row r="1" spans="1:23" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -6212,6 +6219,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6219,8 +6227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6228,124 +6236,112 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>46</v>
+    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>47</v>
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="5">
@@ -6358,8 +6354,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
@@ -6369,8 +6365,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="6">
@@ -6381,7 +6377,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B17">
@@ -6433,16 +6429,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>45</v>
+      <c r="A1" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>42</v>

</xml_diff>